<commit_message>
4Q266 Frag. 1 c b refactored
</commit_message>
<xml_diff>
--- a/Digital_Editions/4Q266/457_1239_Frg_1_c/457_1239_b/457_1239_b.xlsx
+++ b/Digital_Editions/4Q266/457_1239_Frg_1_c/457_1239_b/457_1239_b.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Tucker-James/github/SQE-Damascus/Digital_Editions/4Q266/457_1239_Frg_1_c/457_1239_b/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07A2029-7423-0642-BA53-0BF2B1B5949D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="13020" windowWidth="38400" windowHeight="8580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHARs" sheetId="1" r:id="rId1"/>
     <sheet name="SIGNs" sheetId="2" r:id="rId2"/>
     <sheet name="Sub_Frags" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -175,13 +189,46 @@
   </si>
   <si>
     <t>02_Frg_1_c_ב_ROI.tif:2568-3087-9:1</t>
+  </si>
+  <si>
+    <t>◦</t>
+  </si>
+  <si>
+    <t>א</t>
+  </si>
+  <si>
+    <t>ש</t>
+  </si>
+  <si>
+    <t>מ</t>
+  </si>
+  <si>
+    <t>ה</t>
+  </si>
+  <si>
+    <t>ת</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>certain</t>
+  </si>
+  <si>
+    <t>probable_letter</t>
+  </si>
+  <si>
+    <t>These are very small fragments crunched together. Based on the disarray of ink shapes, these small fragments are likely misplaced. This fragment appears like this in all the PAM plates.</t>
+  </si>
+  <si>
+    <t>DAMAGED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +265,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +319,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,9 +351,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,6 +403,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,17 +596,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,438 +683,381 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C2">
         <f>SIGNs!A2</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
       </c>
       <c r="P2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C3">
         <f>SIGNs!A3</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>59</v>
       </c>
       <c r="P3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C4">
         <f>SIGNs!A4</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>59</v>
       </c>
       <c r="P4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" t="s">
+        <v>63</v>
+      </c>
+      <c r="X4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C5">
         <f>SIGNs!A5</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="Q5" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" t="s">
+        <v>63</v>
+      </c>
+      <c r="X5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C6">
         <f>SIGNs!A6</f>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>60</v>
       </c>
       <c r="P6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>63</v>
+      </c>
+      <c r="W6" t="s">
+        <v>63</v>
+      </c>
+      <c r="X6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C7">
         <f>SIGNs!A7</f>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>60</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="Q7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C8">
         <f>SIGNs!A8</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>61</v>
       </c>
       <c r="P8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>56</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
+        <v>63</v>
+      </c>
+      <c r="W8" t="s">
+        <v>63</v>
+      </c>
+      <c r="X8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C9">
         <f>SIGNs!A9</f>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>61</v>
       </c>
       <c r="P9">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W9" t="s">
+        <v>63</v>
+      </c>
+      <c r="X9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C10">
         <f>SIGNs!A10</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>61</v>
       </c>
       <c r="P10">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R10" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10" t="s">
+        <v>63</v>
+      </c>
+      <c r="W10" t="s">
+        <v>63</v>
+      </c>
+      <c r="X10" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="117">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N10 K1:L10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"null,True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O9" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"null,certain,probable_letter,possible_letter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:X10" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O4">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V4">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W4">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X4">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R4">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W5">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V6">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W6">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X6">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q6">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R6">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S6">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T6">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M7">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V7">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q7">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N8">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V8">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W8">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X8">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q8">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R8">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T8">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9">
-      <formula1>"transformed,reinked,retraced,reinked?,retraced?,intralinear,creased,erased"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9">
-      <formula1>"null,False,True,relevant_w,relevant_h"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9">
-      <formula1>"null,True,False"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9">
-      <formula1>"null,certain,probable_letter,possible_letter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V9">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W9">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X9">
-      <formula1>"DAMAGED,DAMAGED_STILL_READ,NOT_DAMAGED"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q9">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R9">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9">
-      <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1:T9" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"א,ב,ג,ד,ה,ו,ז,ח,ט,י,כ,ך,ל,מ,ם,נ,ן,ס,ע,פ,ף,צ,ץ,ק,ר,ש,ת,◦,l,s,m"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1032,7 +1066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1040,9 +1074,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1098,7 +1132,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1109,7 +1143,7 @@
         <v>2622</v>
       </c>
       <c r="F2">
-        <v>30.836</v>
+        <v>30.835999999999999</v>
       </c>
       <c r="G2">
         <v>11</v>
@@ -1130,25 +1164,25 @@
         <v>57</v>
       </c>
       <c r="M2">
-        <v>64.318</v>
+        <v>64.317999999999998</v>
       </c>
       <c r="N2">
-        <v>51.905</v>
+        <v>51.905000000000001</v>
       </c>
       <c r="O2">
-        <v>0.776</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="P2">
-        <v>1.239</v>
+        <v>1.2390000000000001</v>
       </c>
       <c r="Q2">
-        <v>0.8070000000000001</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1159,7 +1193,7 @@
         <v>3861</v>
       </c>
       <c r="F3">
-        <v>29.097</v>
+        <v>29.097000000000001</v>
       </c>
       <c r="G3">
         <v>10</v>
@@ -1183,22 +1217,22 @@
         <v>111.71</v>
       </c>
       <c r="N3">
-        <v>44.007</v>
+        <v>44.006999999999998</v>
       </c>
       <c r="O3">
-        <v>0.637</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="P3">
-        <v>2.538</v>
+        <v>2.5379999999999998</v>
       </c>
       <c r="Q3">
-        <v>0.394</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1209,7 +1243,7 @@
         <v>2520</v>
       </c>
       <c r="F4">
-        <v>45.515</v>
+        <v>45.515000000000001</v>
       </c>
       <c r="G4">
         <v>13</v>
@@ -1230,10 +1264,10 @@
         <v>63</v>
       </c>
       <c r="M4">
-        <v>71.08799999999999</v>
+        <v>71.087999999999994</v>
       </c>
       <c r="N4">
-        <v>45.135</v>
+        <v>45.134999999999998</v>
       </c>
       <c r="O4">
         <v>0.746</v>
@@ -1242,13 +1276,13 @@
         <v>1.575</v>
       </c>
       <c r="Q4">
-        <v>0.635</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="R4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1259,7 +1293,7 @@
         <v>31486</v>
       </c>
       <c r="F5">
-        <v>42.115</v>
+        <v>42.115000000000002</v>
       </c>
       <c r="G5">
         <v>9</v>
@@ -1280,25 +1314,25 @@
         <v>173</v>
       </c>
       <c r="M5">
-        <v>205.365</v>
+        <v>205.36500000000001</v>
       </c>
       <c r="N5">
         <v>195.21</v>
       </c>
       <c r="O5">
-        <v>0.785</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="P5">
         <v>1.052</v>
       </c>
       <c r="Q5">
-        <v>0.951</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="R5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1309,7 +1343,7 @@
         <v>30960</v>
       </c>
       <c r="F6">
-        <v>34.654</v>
+        <v>34.654000000000003</v>
       </c>
       <c r="G6">
         <v>9</v>
@@ -1333,22 +1367,22 @@
         <v>203.108</v>
       </c>
       <c r="N6">
-        <v>194.081</v>
+        <v>194.08099999999999</v>
       </c>
       <c r="O6">
-        <v>0.785</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="P6">
-        <v>1.047</v>
+        <v>1.0469999999999999</v>
       </c>
       <c r="Q6">
-        <v>0.956</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1359,7 +1393,7 @@
         <v>31073</v>
       </c>
       <c r="F7">
-        <v>27.455</v>
+        <v>27.454999999999998</v>
       </c>
       <c r="G7">
         <v>7</v>
@@ -1380,25 +1414,25 @@
         <v>161</v>
       </c>
       <c r="M7">
-        <v>217.777</v>
+        <v>217.77699999999999</v>
       </c>
       <c r="N7">
-        <v>181.669</v>
+        <v>181.66900000000001</v>
       </c>
       <c r="O7">
-        <v>0.779</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="P7">
-        <v>1.199</v>
+        <v>1.1990000000000001</v>
       </c>
       <c r="Q7">
-        <v>0.834</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="R7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1409,7 +1443,7 @@
         <v>9102</v>
       </c>
       <c r="F8">
-        <v>18.066</v>
+        <v>18.065999999999999</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -1433,22 +1467,22 @@
         <v>125.25</v>
       </c>
       <c r="N8">
-        <v>92.527</v>
+        <v>92.527000000000001</v>
       </c>
       <c r="O8">
-        <v>0.768</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="P8">
-        <v>1.354</v>
+        <v>1.3540000000000001</v>
       </c>
       <c r="Q8">
-        <v>0.739</v>
+        <v>0.73899999999999999</v>
       </c>
       <c r="R8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1483,22 +1517,22 @@
         <v>126.378</v>
       </c>
       <c r="N9">
-        <v>69.95999999999999</v>
+        <v>69.959999999999994</v>
       </c>
       <c r="O9">
-        <v>0.721</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="P9">
         <v>1.806</v>
       </c>
       <c r="Q9">
-        <v>0.554</v>
+        <v>0.55400000000000005</v>
       </c>
       <c r="R9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1509,7 +1543,7 @@
         <v>6336</v>
       </c>
       <c r="F10">
-        <v>22.533</v>
+        <v>22.533000000000001</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -1533,16 +1567,16 @@
         <v>108.324</v>
       </c>
       <c r="N10">
-        <v>74.473</v>
+        <v>74.472999999999999</v>
       </c>
       <c r="O10">
-        <v>0.758</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="P10">
-        <v>1.455</v>
+        <v>1.4550000000000001</v>
       </c>
       <c r="Q10">
-        <v>0.6879999999999999</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1554,14 +1588,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>

</xml_diff>